<commit_message>
WRI edits for BESP
</commit_message>
<xml_diff>
--- a/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
+++ b/InputData/trans/BESP/BAU EV Subsidy Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS\Input Data for India 2.0\trans\BESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0162AE8-90DA-4C3C-A988-E237791EE209}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8DB12C8-F065-437B-99AD-5447280A3DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,15 @@
     <sheet name="BESP-passengers" sheetId="3" r:id="rId6"/>
     <sheet name="BESP-freight" sheetId="4" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="160">
   <si>
     <t>BESP BAU EV Subsidy Percentage</t>
   </si>
@@ -193,24 +196,12 @@
 (incl. e-rickshaws)</t>
   </si>
   <si>
-    <t>e-4 wheelers</t>
-  </si>
-  <si>
     <t>4W strong hybrid vehicle</t>
   </si>
   <si>
     <t>e-bus</t>
   </si>
   <si>
-    <t>Total approximate incentive @Rs. 10000/kWh for all vehicles</t>
-  </si>
-  <si>
-    <t>and Rs. 20000/kWh for buses and trucks</t>
-  </si>
-  <si>
-    <t>Incentives for BEVs (FAME I)</t>
-  </si>
-  <si>
     <t>Incentives for BEVs (FAME II)</t>
   </si>
   <si>
@@ -223,27 +214,9 @@
     <t>Notification on Phase-II of FAME India Scheme</t>
   </si>
   <si>
-    <t>Passengers</t>
-  </si>
-  <si>
-    <t>Freight</t>
-  </si>
-  <si>
     <t>EPS category</t>
   </si>
   <si>
-    <t>Motorbike - freight</t>
-  </si>
-  <si>
-    <t>LDVs - passenger</t>
-  </si>
-  <si>
-    <t>Motorbike - passenger</t>
-  </si>
-  <si>
-    <t>HDVs - passenger</t>
-  </si>
-  <si>
     <t>Price ($/vehicle)</t>
   </si>
   <si>
@@ -457,15 +430,9 @@
     <t>Max Ex-factory price to avail incentives</t>
   </si>
   <si>
-    <t xml:space="preserve">From 2020 onward, FAME II incentive rates are used. FAME II has caps on max available </t>
-  </si>
-  <si>
     <t>subsidy as a percentage of price for buses and other categories.</t>
   </si>
   <si>
-    <t>Passenger LDVs</t>
-  </si>
-  <si>
     <t>Passenger HDVs</t>
   </si>
   <si>
@@ -484,37 +451,84 @@
     <t>India’s Energy Transition:  Subsidies for Fossil Fuels and Renewable Energy</t>
   </si>
   <si>
-    <t>LDVs - freight</t>
-  </si>
-  <si>
     <t>Freight LDVs</t>
   </si>
   <si>
-    <t>Subsidy %</t>
-  </si>
-  <si>
-    <t>Cap on subsidies for buses</t>
-  </si>
-  <si>
     <t>Cap for remaining vehicles</t>
   </si>
   <si>
     <t>Till 2018, FAME I scheme incentives are used.</t>
   </si>
   <si>
-    <t>Subsidy period - 3 years -  (2019, '20, '21)</t>
+    <t>and Rs. 20000/kWh for buses and trucks.</t>
+  </si>
+  <si>
+    <t>Cap on subsidies for buses and 2 wheelers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incentives for BEVs (FAME I) </t>
+  </si>
+  <si>
+    <t>FAME II Update</t>
+  </si>
+  <si>
+    <t>Press Information Bureau, Govt. of India</t>
+  </si>
+  <si>
+    <t>Year-End- Review of Ministry of Heavy Industries – 2021</t>
+  </si>
+  <si>
+    <t>https://pib.gov.in/pressreleasepage.aspx?prid=1784161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 2019 onward, FAME II incentive rates are used. FAME II has caps on max available </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> From 2022 onward, updates made to the FAME II incentive rates in 2021 are considered.</t>
+  </si>
+  <si>
+    <t>commercial e-4 wheelers (taxis)</t>
+  </si>
+  <si>
+    <t>Total approximate incentive @Rs. 10000/kWh for 4 wheelers;</t>
+  </si>
+  <si>
+    <t>Rs 10,000/kWh from 2019-2021 and 15,000/Kwh from 2022-2024 for 2 wheelers;</t>
+  </si>
+  <si>
+    <t>Incentives for all 2 wheelers, and public and commercial vehicles in other vehicle categories.</t>
+  </si>
+  <si>
+    <t>Subsidy (2019, '20, '21) %</t>
+  </si>
+  <si>
+    <t>Subsidy (2022, '23, '24) %</t>
+  </si>
+  <si>
+    <t>Incentive/vehicle (2019-21)</t>
+  </si>
+  <si>
+    <t>Incentive/vehicle (2022-24)</t>
+  </si>
+  <si>
+    <t>EPS Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passenger ships </t>
+  </si>
+  <si>
+    <t>Passenger ships (repuposed as taxis for India)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +566,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -573,7 +594,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -581,84 +602,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -714,22 +664,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -737,20 +676,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1191,9 +1137,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1211,7 +1159,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>40</v>
@@ -1219,7 +1167,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
         <v>41</v>
@@ -1238,7 +1186,7 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,12 +1210,12 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,175 +1225,197 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="29" t="s">
-        <v>59</v>
+      <c r="D14" s="28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="17"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="17"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="17"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="35">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="17"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B22" s="17"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B23" s="17"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B24" s="17"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>148</v>
+      </c>
       <c r="B25" s="17"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="17"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="17"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
       <c r="B27" s="17"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="17"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
-      <c r="B28"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="B29"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>36</v>
       </c>
-      <c r="B30"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B31"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B32"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>66.319999999999993</v>
-      </c>
-      <c r="B33" s="2">
-        <v>2015</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>137</v>
-      </c>
+      <c r="B33"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>66.319999999999993</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>68.66</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B35" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B35"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>10000000</v>
       </c>
-      <c r="B36"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B38"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>100000</v>
       </c>
-      <c r="B39"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="B40"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42"/>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="27"/>
       <c r="B43"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D14" r:id="rId2" xr:uid="{CE9DCEEF-D2EF-4EE5-A687-805E90B8B0AB}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{05A9072E-98B4-4505-B697-14241F072907}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1453,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7610541F-3EBC-4549-936B-7E451B157FAE}">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,64 +1435,64 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>34.799999999999997</v>
@@ -1536,13 +1506,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>36.700000000000003</v>
@@ -1556,13 +1526,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>38.799999999999997</v>
@@ -1576,13 +1546,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D10">
         <v>40.5</v>
@@ -1596,13 +1566,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>41.8</v>
@@ -1616,13 +1586,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>44.4</v>
@@ -1636,13 +1606,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D13">
         <v>49.3</v>
@@ -1656,13 +1626,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>53.8</v>
@@ -1676,13 +1646,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>56.9</v>
@@ -1696,13 +1666,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>60.6</v>
@@ -1716,13 +1686,13 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D17">
         <v>65.2</v>
@@ -1736,13 +1706,13 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D18">
         <v>72.599999999999994</v>
@@ -1756,13 +1726,13 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D19">
         <v>82.4</v>
@@ -1776,13 +1746,13 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D20">
         <v>90.9</v>
@@ -1796,13 +1766,13 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D21">
         <v>96.5</v>
@@ -1816,13 +1786,13 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D22">
         <v>99.6</v>
@@ -1836,7 +1806,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>102.9</v>
@@ -1856,7 +1826,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>106.6</v>
@@ -1876,7 +1846,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B25">
         <v>109.1</v>
@@ -1896,7 +1866,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B26">
         <v>112.4</v>
@@ -1916,7 +1886,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B27">
         <v>116.8</v>
@@ -1936,7 +1906,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <v>122.7</v>
@@ -1956,7 +1926,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B29">
         <v>128.69999999999999</v>
@@ -1980,7 +1950,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B30">
         <v>135.19999999999999</v>
@@ -2007,7 +1977,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B31">
         <v>139.19999999999999</v>
@@ -2034,7 +2004,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B32">
         <v>143.69999999999999</v>
@@ -2061,7 +2031,7 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B33">
         <v>147.19999999999999</v>
@@ -2088,7 +2058,7 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B34">
         <v>151.5</v>
@@ -2115,7 +2085,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B35">
         <v>155.80000000000001</v>
@@ -2142,7 +2112,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B36">
         <v>159.9</v>
@@ -2169,7 +2139,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B37">
         <v>162.30000000000001</v>
@@ -2196,7 +2166,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B38">
         <v>165.4</v>
@@ -2223,7 +2193,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B39">
         <v>170.8</v>
@@ -2250,7 +2220,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B40">
         <v>176.6</v>
@@ -2277,7 +2247,7 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B41">
         <v>178.9</v>
@@ -2304,7 +2274,7 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B42">
         <v>183.3</v>
@@ -2331,7 +2301,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B43">
         <v>187.6</v>
@@ -2358,7 +2328,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B44">
         <v>193.2</v>
@@ -2385,7 +2355,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B45">
         <v>200.6</v>
@@ -2412,7 +2382,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B46">
         <v>205.709</v>
@@ -2439,7 +2409,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B47">
         <v>214.429</v>
@@ -2466,7 +2436,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B48">
         <v>213.13900000000001</v>
@@ -2493,7 +2463,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B49">
         <v>217.535</v>
@@ -2520,7 +2490,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B50">
         <v>223.59800000000001</v>
@@ -2547,7 +2517,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B51">
         <v>228.85</v>
@@ -2574,7 +2544,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B52">
         <v>232.36600000000001</v>
@@ -2601,7 +2571,7 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B53">
         <v>236.38399999999999</v>
@@ -2628,7 +2598,7 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B54">
         <v>236.26499999999999</v>
@@ -2655,7 +2625,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B55">
         <v>238.77799999999999</v>
@@ -2682,7 +2652,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B56">
         <v>244.07599999999999</v>
@@ -2709,7 +2679,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B57">
         <v>250.089</v>
@@ -2790,10 +2760,10 @@
       <c r="F77" s="15"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="34" t="s">
+      <c r="B78" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="35"/>
+      <c r="C78" s="39"/>
       <c r="D78" s="13" t="s">
         <v>29</v>
       </c>
@@ -2839,7 +2809,7 @@
         <v>17500</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2847,19 +2817,19 @@
         <v>10</v>
       </c>
       <c r="B81" s="12">
-        <f>(B80/About!$A$33)*'US CPI Data'!$G$54</f>
+        <f>(B80/About!$A$34)*'US CPI Data'!$G$54</f>
         <v>1453.3144805597994</v>
       </c>
       <c r="C81" s="12">
-        <f>(C80/About!$A$33)*'US CPI Data'!$G$54</f>
+        <f>(C80/About!$A$34)*'US CPI Data'!$G$54</f>
         <v>2070.4254032095637</v>
       </c>
       <c r="D81" s="12">
-        <f>(D80/About!$A$33)*'US CPI Data'!$G$54</f>
+        <f>(D80/About!$A$34)*'US CPI Data'!$G$54</f>
         <v>140.58444095867409</v>
       </c>
       <c r="E81" s="12">
-        <f>(E80/About!$A$33)*'US CPI Data'!$G$54</f>
+        <f>(E80/About!$A$34)*'US CPI Data'!$G$54</f>
         <v>255.60807447031652</v>
       </c>
       <c r="F81" s="8" t="s">
@@ -2878,17 +2848,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E86C2E-D775-44A4-A1DD-3ACC1483F778}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
@@ -2900,295 +2870,257 @@
         <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" t="s">
-        <v>139</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="F3" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" s="22"/>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4">
-        <v>20000</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4">
-        <v>150000</v>
-      </c>
-      <c r="I4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5">
-        <v>50000</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5">
-        <v>500000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>65</v>
+      <c r="B4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6">
-        <v>150000</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6">
-        <v>1500000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>66</v>
+      <c r="B6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7">
-        <v>13000</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7">
-        <f>F6</f>
-        <v>1500000</v>
-      </c>
-      <c r="I7" t="s">
-        <v>149</v>
-      </c>
+      <c r="B7" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="F7" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>5000000</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>20000</v>
+      </c>
+      <c r="C8" s="6">
+        <v>30000</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8">
-        <v>20000000</v>
+        <v>150000</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="41"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>50000</v>
+      </c>
+      <c r="C9" s="6">
+        <v>50000</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9">
+        <v>500000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10">
+        <v>150000</v>
+      </c>
+      <c r="C10" s="6">
+        <v>150000</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10">
+        <v>1500000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>13000</v>
+      </c>
+      <c r="C11" s="6">
+        <v>13000</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11">
+        <f>F10</f>
+        <v>1500000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="32">
-        <f>B6/F6</f>
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>5000000</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5000000</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12">
+        <v>20000000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="33">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="36">
+        <f>B10/$F10</f>
         <v>0.1</v>
       </c>
-      <c r="C12" s="43">
-        <f>B7/F7</f>
+      <c r="C18" s="36">
+        <f>C10/F10</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="36">
+        <f>B12/F12</f>
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="36">
+        <f>C12/F12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="36">
+        <f>B8/F8</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="C20" s="36">
+        <f>C8/F8</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="36">
+        <f>B11/F11</f>
         <v>8.6666666666666663E-3</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37" t="s">
-        <v>152</v>
-      </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="46">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="32">
-        <f>B8/F8</f>
-        <v>0.25</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="46">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="33">
-        <f>B4/F4</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="C17" s="45">
-        <f>B5/F5</f>
+      <c r="C21" s="36">
+        <f>C11/$F11</f>
+        <v>8.6666666666666663E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="36">
+        <f>B9/F9</f>
         <v>0.1</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B21">
-        <f>B12</f>
+      <c r="C22" s="36">
+        <f>C9/F9</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22">
-        <f>B13</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" s="27">
-        <f>B17</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="C23" s="27"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" s="47">
-        <f>C12</f>
-        <v>8.6666666666666663E-3</v>
-      </c>
-      <c r="C24" s="27"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25">
-        <f>C17</f>
-        <v>0.1</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
+  <mergeCells count="1">
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3220,7 +3152,7 @@
     </row>
     <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>15</v>
@@ -3340,7 +3272,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -3360,7 +3292,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -3392,7 +3324,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3332,7 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>47</v>
       </c>
@@ -3523,134 +3455,135 @@
         <v>0.12013036760839702</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:E2" si="0">$B2</f>
+        <f t="shared" ref="D2" si="0">$B2</f>
         <v>0.12013036760839702</v>
       </c>
-      <c r="E2" s="5">
-        <f>'FAME II subsidies'!B21</f>
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="5">
-        <f>E2</f>
-        <v>0.1</v>
-      </c>
-      <c r="G2" s="5">
-        <f t="shared" ref="G2:H2" si="1">F2</f>
-        <v>0.1</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
-        <f>'FAME II subsidies'!F21</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="5">
-        <f>'FAME II subsidies'!G21</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="5">
-        <f>'FAME II subsidies'!H21</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="5">
-        <f>'FAME II subsidies'!I21</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="5">
-        <f>'FAME II subsidies'!J21</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="5">
-        <f>'FAME II subsidies'!K21</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="5">
-        <f>'FAME II subsidies'!L21</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="5">
-        <f>'FAME II subsidies'!M21</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <f>'FAME II subsidies'!N21</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <f>'FAME II subsidies'!O21</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <f>'FAME II subsidies'!P21</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
-        <f>'FAME II subsidies'!Q21</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <f>'FAME II subsidies'!R21</f>
-        <v>0</v>
-      </c>
-      <c r="V2" s="5">
-        <f>'FAME II subsidies'!S21</f>
-        <v>0</v>
-      </c>
-      <c r="W2" s="5">
-        <f>'FAME II subsidies'!T21</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="5">
-        <f>'FAME II subsidies'!U21</f>
-        <v>0</v>
-      </c>
-      <c r="Y2" s="5">
-        <f>'FAME II subsidies'!V21</f>
-        <v>0</v>
-      </c>
-      <c r="Z2" s="5">
-        <f>'FAME II subsidies'!W21</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="5">
-        <f>'FAME II subsidies'!X21</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="5">
-        <f>'FAME II subsidies'!Y21</f>
-        <v>0</v>
-      </c>
-      <c r="AC2" s="5">
-        <f>'FAME II subsidies'!Z21</f>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="5">
-        <f>'FAME II subsidies'!AA21</f>
-        <v>0</v>
-      </c>
-      <c r="AE2" s="5">
-        <f>'FAME II subsidies'!AB21</f>
-        <v>0</v>
-      </c>
-      <c r="AF2" s="5">
-        <f>'FAME II subsidies'!AC21</f>
-        <v>0</v>
-      </c>
-      <c r="AG2" s="5">
-        <f>'FAME II subsidies'!AD21</f>
-        <v>0</v>
-      </c>
-      <c r="AH2" s="5">
-        <f>'FAME II subsidies'!AE21</f>
-        <v>0</v>
-      </c>
-      <c r="AI2" s="5">
-        <f>'FAME II subsidies'!AF21</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="5">
-        <f>'FAME II subsidies'!AG21</f>
+      <c r="E2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AG2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="37">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="37">
+        <f>0</f>
         <v>0</v>
       </c>
     </row>
@@ -3667,132 +3600,132 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <f>'FAME II subsidies'!B22</f>
+      <c r="E3" s="34">
+        <f>'FAME II subsidies'!$B$19</f>
         <v>0.25</v>
       </c>
-      <c r="F3">
-        <f>E3</f>
+      <c r="F3" s="34">
+        <f>'FAME II subsidies'!$B$19</f>
         <v>0.25</v>
       </c>
-      <c r="G3">
-        <f>F3</f>
+      <c r="G3" s="34">
+        <f>'FAME II subsidies'!$B$19</f>
         <v>0.25</v>
       </c>
-      <c r="H3">
-        <f>'FAME II subsidies'!E22</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f>'FAME II subsidies'!F22</f>
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <f>'FAME II subsidies'!G22</f>
-        <v>0</v>
+      <c r="H3" s="34">
+        <f>'FAME II subsidies'!$C$19</f>
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="34">
+        <f>'FAME II subsidies'!$C$19</f>
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="34">
+        <f>'FAME II subsidies'!$C$19</f>
+        <v>0.25</v>
       </c>
       <c r="K3">
-        <f>'FAME II subsidies'!H22</f>
+        <f>'FAME II subsidies'!H19</f>
         <v>0</v>
       </c>
       <c r="L3">
-        <f>'FAME II subsidies'!I22</f>
+        <f>'FAME II subsidies'!I19</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>'FAME II subsidies'!J22</f>
+        <f>'FAME II subsidies'!J19</f>
         <v>0</v>
       </c>
       <c r="N3">
-        <f>'FAME II subsidies'!K22</f>
+        <f>'FAME II subsidies'!K19</f>
         <v>0</v>
       </c>
       <c r="O3">
-        <f>'FAME II subsidies'!L22</f>
+        <f>'FAME II subsidies'!L19</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f>'FAME II subsidies'!M22</f>
+        <f>'FAME II subsidies'!M19</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f>'FAME II subsidies'!N22</f>
+        <f>'FAME II subsidies'!N19</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f>'FAME II subsidies'!O22</f>
+        <f>'FAME II subsidies'!O19</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f>'FAME II subsidies'!P22</f>
+        <f>'FAME II subsidies'!P19</f>
         <v>0</v>
       </c>
       <c r="T3">
-        <f>'FAME II subsidies'!Q22</f>
+        <f>'FAME II subsidies'!Q19</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f>'FAME II subsidies'!R22</f>
+        <f>'FAME II subsidies'!R19</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f>'FAME II subsidies'!S22</f>
+        <f>'FAME II subsidies'!S19</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f>'FAME II subsidies'!T22</f>
+        <f>'FAME II subsidies'!T19</f>
         <v>0</v>
       </c>
       <c r="X3">
-        <f>'FAME II subsidies'!U22</f>
+        <f>'FAME II subsidies'!U19</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f>'FAME II subsidies'!V22</f>
+        <f>'FAME II subsidies'!V19</f>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f>'FAME II subsidies'!W22</f>
+        <f>'FAME II subsidies'!W19</f>
         <v>0</v>
       </c>
       <c r="AA3">
-        <f>'FAME II subsidies'!X22</f>
+        <f>'FAME II subsidies'!X19</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f>'FAME II subsidies'!Y22</f>
+        <f>'FAME II subsidies'!Y19</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f>'FAME II subsidies'!Z22</f>
+        <f>'FAME II subsidies'!Z19</f>
         <v>0</v>
       </c>
       <c r="AD3">
-        <f>'FAME II subsidies'!AA22</f>
+        <f>'FAME II subsidies'!AA19</f>
         <v>0</v>
       </c>
       <c r="AE3">
-        <f>'FAME II subsidies'!AB22</f>
+        <f>'FAME II subsidies'!AB19</f>
         <v>0</v>
       </c>
       <c r="AF3">
-        <f>'FAME II subsidies'!AC22</f>
+        <f>'FAME II subsidies'!AC19</f>
         <v>0</v>
       </c>
       <c r="AG3">
-        <f>'FAME II subsidies'!AD22</f>
+        <f>'FAME II subsidies'!AD19</f>
         <v>0</v>
       </c>
       <c r="AH3">
-        <f>'FAME II subsidies'!AE22</f>
+        <f>'FAME II subsidies'!AE19</f>
         <v>0</v>
       </c>
       <c r="AI3">
-        <f>'FAME II subsidies'!AF22</f>
+        <f>'FAME II subsidies'!AF19</f>
         <v>0</v>
       </c>
       <c r="AJ3">
-        <f>'FAME II subsidies'!AG22</f>
+        <f>'FAME II subsidies'!AG19</f>
         <v>0</v>
       </c>
     </row>
@@ -4029,23 +3962,29 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
+      <c r="E6" s="34">
+        <f>'FAME II subsidies'!$B$18</f>
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="34">
+        <f>'FAME II subsidies'!$B$18</f>
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="34">
+        <f>'FAME II subsidies'!$B$18</f>
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="34">
+        <f>'FAME II subsidies'!$C$18</f>
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="34">
+        <f>'FAME II subsidies'!$C$18</f>
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="34">
+        <f>'FAME II subsidies'!$C$18</f>
+        <v>0.1</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -4139,135 +4078,135 @@
         <v>0.24184497685740278</v>
       </c>
       <c r="D7" s="5">
-        <f t="shared" ref="D7:E7" si="2">$B7</f>
+        <f t="shared" ref="D7" si="1">$B7</f>
         <v>0.24184497685740278</v>
       </c>
       <c r="E7" s="5">
-        <f>'FAME II subsidies'!B23</f>
+        <f>'FAME II subsidies'!$B$20</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="F7" s="5">
-        <f>E7</f>
+        <f>'FAME II subsidies'!$B$20</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="G7" s="5">
-        <f>F7</f>
+        <f>'FAME II subsidies'!$B$20</f>
         <v>0.13333333333333333</v>
       </c>
       <c r="H7" s="5">
-        <f>'FAME II subsidies'!E23</f>
-        <v>0</v>
+        <f>'FAME II subsidies'!$C$20</f>
+        <v>0.2</v>
       </c>
       <c r="I7" s="5">
-        <f>'FAME II subsidies'!F23</f>
-        <v>0</v>
+        <f>'FAME II subsidies'!$C$20</f>
+        <v>0.2</v>
       </c>
       <c r="J7" s="5">
-        <f>'FAME II subsidies'!G23</f>
-        <v>0</v>
+        <f>'FAME II subsidies'!$C$20</f>
+        <v>0.2</v>
       </c>
       <c r="K7" s="5">
-        <f>'FAME II subsidies'!H23</f>
+        <f>'FAME II subsidies'!H20</f>
         <v>0</v>
       </c>
       <c r="L7" s="5">
-        <f>'FAME II subsidies'!I23</f>
+        <f>'FAME II subsidies'!I20</f>
         <v>0</v>
       </c>
       <c r="M7" s="5">
-        <f>'FAME II subsidies'!J23</f>
+        <f>'FAME II subsidies'!J20</f>
         <v>0</v>
       </c>
       <c r="N7" s="5">
-        <f>'FAME II subsidies'!K23</f>
+        <f>'FAME II subsidies'!K20</f>
         <v>0</v>
       </c>
       <c r="O7" s="5">
-        <f>'FAME II subsidies'!L23</f>
+        <f>'FAME II subsidies'!L20</f>
         <v>0</v>
       </c>
       <c r="P7" s="5">
-        <f>'FAME II subsidies'!M23</f>
+        <f>'FAME II subsidies'!M20</f>
         <v>0</v>
       </c>
       <c r="Q7" s="5">
-        <f>'FAME II subsidies'!N23</f>
+        <f>'FAME II subsidies'!N20</f>
         <v>0</v>
       </c>
       <c r="R7" s="5">
-        <f>'FAME II subsidies'!O23</f>
+        <f>'FAME II subsidies'!O20</f>
         <v>0</v>
       </c>
       <c r="S7" s="5">
-        <f>'FAME II subsidies'!P23</f>
+        <f>'FAME II subsidies'!P20</f>
         <v>0</v>
       </c>
       <c r="T7" s="5">
-        <f>'FAME II subsidies'!Q23</f>
+        <f>'FAME II subsidies'!Q20</f>
         <v>0</v>
       </c>
       <c r="U7" s="5">
-        <f>'FAME II subsidies'!R23</f>
+        <f>'FAME II subsidies'!R20</f>
         <v>0</v>
       </c>
       <c r="V7" s="5">
-        <f>'FAME II subsidies'!S23</f>
+        <f>'FAME II subsidies'!S20</f>
         <v>0</v>
       </c>
       <c r="W7" s="5">
-        <f>'FAME II subsidies'!T23</f>
+        <f>'FAME II subsidies'!T20</f>
         <v>0</v>
       </c>
       <c r="X7" s="5">
-        <f>'FAME II subsidies'!U23</f>
+        <f>'FAME II subsidies'!U20</f>
         <v>0</v>
       </c>
       <c r="Y7" s="5">
-        <f>'FAME II subsidies'!V23</f>
+        <f>'FAME II subsidies'!V20</f>
         <v>0</v>
       </c>
       <c r="Z7" s="5">
-        <f>'FAME II subsidies'!W23</f>
+        <f>'FAME II subsidies'!W20</f>
         <v>0</v>
       </c>
       <c r="AA7" s="5">
-        <f>'FAME II subsidies'!X23</f>
+        <f>'FAME II subsidies'!X20</f>
         <v>0</v>
       </c>
       <c r="AB7" s="5">
-        <f>'FAME II subsidies'!Y23</f>
+        <f>'FAME II subsidies'!Y20</f>
         <v>0</v>
       </c>
       <c r="AC7" s="5">
-        <f>'FAME II subsidies'!Z23</f>
+        <f>'FAME II subsidies'!Z20</f>
         <v>0</v>
       </c>
       <c r="AD7" s="5">
-        <f>'FAME II subsidies'!AA23</f>
+        <f>'FAME II subsidies'!AA20</f>
         <v>0</v>
       </c>
       <c r="AE7" s="5">
-        <f>'FAME II subsidies'!AB23</f>
+        <f>'FAME II subsidies'!AB20</f>
         <v>0</v>
       </c>
       <c r="AF7" s="5">
-        <f>'FAME II subsidies'!AC23</f>
+        <f>'FAME II subsidies'!AC20</f>
         <v>0</v>
       </c>
       <c r="AG7" s="5">
-        <f>'FAME II subsidies'!AD23</f>
+        <f>'FAME II subsidies'!AD20</f>
         <v>0</v>
       </c>
       <c r="AH7" s="5">
-        <f>'FAME II subsidies'!AE23</f>
+        <f>'FAME II subsidies'!AE20</f>
         <v>0</v>
       </c>
       <c r="AI7" s="5">
-        <f>'FAME II subsidies'!AF23</f>
+        <f>'FAME II subsidies'!AF20</f>
         <v>0</v>
       </c>
       <c r="AJ7" s="5">
-        <f>'FAME II subsidies'!AG23</f>
+        <f>'FAME II subsidies'!AG20</f>
         <v>0</v>
       </c>
     </row>
@@ -4283,8 +4222,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4231,7 @@
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>47</v>
       </c>
@@ -4415,26 +4354,29 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="47">
-        <f>'FAME II subsidies'!B24</f>
+      <c r="E2" s="34">
+        <f>'FAME II subsidies'!$B$21</f>
         <v>8.6666666666666663E-3</v>
       </c>
-      <c r="F2" s="47">
-        <f>E2</f>
+      <c r="F2" s="34">
+        <f>'FAME II subsidies'!$B$21</f>
         <v>8.6666666666666663E-3</v>
       </c>
-      <c r="G2" s="47">
-        <f>F2</f>
+      <c r="G2" s="34">
+        <f>'FAME II subsidies'!$B$21</f>
         <v>8.6666666666666663E-3</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="H2" s="34">
+        <f>'FAME II subsidies'!$C$21</f>
+        <v>8.6666666666666663E-3</v>
+      </c>
+      <c r="I2" s="34">
+        <f>'FAME II subsidies'!$C$21</f>
+        <v>8.6666666666666663E-3</v>
+      </c>
+      <c r="J2" s="34">
+        <f>'FAME II subsidies'!$C$21</f>
+        <v>8.6666666666666663E-3</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4964,7 +4906,7 @@
         <v>0.18653952686712924</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" ref="C7:E7" si="0">$B7</f>
+        <f t="shared" ref="C7:D7" si="0">$B7</f>
         <v>0.18653952686712924</v>
       </c>
       <c r="D7" s="5">
@@ -4972,131 +4914,131 @@
         <v>0.18653952686712924</v>
       </c>
       <c r="E7" s="5">
-        <f>'FAME II subsidies'!B25</f>
+        <f>'FAME II subsidies'!$B$22</f>
         <v>0.1</v>
       </c>
       <c r="F7" s="5">
-        <f>E7</f>
+        <f>'FAME II subsidies'!$B$22</f>
         <v>0.1</v>
       </c>
       <c r="G7" s="5">
-        <f>F7</f>
+        <f>'FAME II subsidies'!$B$22</f>
         <v>0.1</v>
       </c>
       <c r="H7" s="5">
-        <f>'FAME II subsidies'!E25</f>
-        <v>0</v>
+        <f>'FAME II subsidies'!$C$22</f>
+        <v>0.1</v>
       </c>
       <c r="I7" s="5">
-        <f>'FAME II subsidies'!F25</f>
-        <v>0</v>
+        <f>'FAME II subsidies'!$C$22</f>
+        <v>0.1</v>
       </c>
       <c r="J7" s="5">
-        <f>'FAME II subsidies'!G25</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <f>'FAME II subsidies'!H25</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <f>'FAME II subsidies'!I25</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="5">
-        <f>'FAME II subsidies'!J25</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <f>'FAME II subsidies'!K25</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <f>'FAME II subsidies'!L25</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <f>'FAME II subsidies'!M25</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <f>'FAME II subsidies'!N25</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="5">
-        <f>'FAME II subsidies'!O25</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="5">
-        <f>'FAME II subsidies'!P25</f>
-        <v>0</v>
-      </c>
-      <c r="T7" s="5">
-        <f>'FAME II subsidies'!Q25</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="5">
-        <f>'FAME II subsidies'!R25</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="5">
-        <f>'FAME II subsidies'!S25</f>
-        <v>0</v>
-      </c>
-      <c r="W7" s="5">
-        <f>'FAME II subsidies'!T25</f>
-        <v>0</v>
-      </c>
-      <c r="X7" s="5">
-        <f>'FAME II subsidies'!U25</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="5">
-        <f>'FAME II subsidies'!V25</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="5">
-        <f>'FAME II subsidies'!W25</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="5">
-        <f>'FAME II subsidies'!X25</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="5">
-        <f>'FAME II subsidies'!Y25</f>
-        <v>0</v>
-      </c>
-      <c r="AC7" s="5">
-        <f>'FAME II subsidies'!Z25</f>
-        <v>0</v>
-      </c>
-      <c r="AD7" s="5">
-        <f>'FAME II subsidies'!AA25</f>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="5">
-        <f>'FAME II subsidies'!AB25</f>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="5">
-        <f>'FAME II subsidies'!AC25</f>
-        <v>0</v>
-      </c>
-      <c r="AG7" s="5">
-        <f>'FAME II subsidies'!AD25</f>
-        <v>0</v>
-      </c>
-      <c r="AH7" s="5">
-        <f>'FAME II subsidies'!AE25</f>
-        <v>0</v>
-      </c>
-      <c r="AI7" s="5">
-        <f>'FAME II subsidies'!AF25</f>
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="5">
-        <f>'FAME II subsidies'!AG25</f>
+        <f>'FAME II subsidies'!$C$22</f>
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="37">
+        <f>'FAME II subsidies'!H22</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="37">
+        <f>'FAME II subsidies'!I22</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="37">
+        <f>'FAME II subsidies'!J22</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="37">
+        <f>'FAME II subsidies'!K22</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="37">
+        <f>'FAME II subsidies'!L22</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="37">
+        <f>'FAME II subsidies'!M22</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="37">
+        <f>'FAME II subsidies'!N22</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="37">
+        <f>'FAME II subsidies'!O22</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="37">
+        <f>'FAME II subsidies'!P22</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="37">
+        <f>'FAME II subsidies'!Q22</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="37">
+        <f>'FAME II subsidies'!R22</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="37">
+        <f>'FAME II subsidies'!S22</f>
+        <v>0</v>
+      </c>
+      <c r="W7" s="37">
+        <f>'FAME II subsidies'!T22</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="37">
+        <f>'FAME II subsidies'!U22</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="37">
+        <f>'FAME II subsidies'!V22</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="37">
+        <f>'FAME II subsidies'!W22</f>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="37">
+        <f>'FAME II subsidies'!X22</f>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="37">
+        <f>'FAME II subsidies'!Y22</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="37">
+        <f>'FAME II subsidies'!Z22</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="37">
+        <f>'FAME II subsidies'!AA22</f>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="37">
+        <f>'FAME II subsidies'!AB22</f>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="37">
+        <f>'FAME II subsidies'!AC22</f>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="37">
+        <f>'FAME II subsidies'!AD22</f>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="37">
+        <f>'FAME II subsidies'!AE22</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="37">
+        <f>'FAME II subsidies'!AF22</f>
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="37">
+        <f>'FAME II subsidies'!AG22</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>